<commit_message>
partial change to step names
</commit_message>
<xml_diff>
--- a/example3/index.xlsx
+++ b/example3/index.xlsx
@@ -50,7 +50,35 @@
     <t xml:space="preserve">conceptsetdataset</t>
   </si>
   <si>
-    <t xml:space="preserve">01_1_T2.1_create_conceptset_datasets</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">01_T2.1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">_1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">_create_conceptset_datasets</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">VACCINES MEDICINES EVENTS SURVEY_OBSERVATIONS MEDICAL_OBSERVATIONS</t>
@@ -65,7 +93,35 @@
     <t xml:space="preserve">output_spells_category</t>
   </si>
   <si>
-    <t xml:space="preserve">01_2_T2.1_create_spells</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">01_T2.1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">_2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">_create_spells</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">OBSERVATION_PERIODS</t>
@@ -80,7 +136,35 @@
     <t xml:space="preserve">D3_PERSONS</t>
   </si>
   <si>
-    <t xml:space="preserve">01_3_T2.1_create_dates_in_PERSONS</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">01_T2.1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">_3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">_create_dates_in_PERSONS</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">PERSONS</t>
@@ -95,7 +179,35 @@
     <t xml:space="preserve">itemsetdataset</t>
   </si>
   <si>
-    <t xml:space="preserve">01_4_T2.1_create_prompt_and_itemset_datasets</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">01_T2.1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">_4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">_create_prompt_and_itemset_datasets</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">SURVEY_OBSERVATIONS MEDICAL_OBSERVATIONS SURVEY_ID VISIT_OCCURRENCE_ID</t>
@@ -113,7 +225,35 @@
     <t xml:space="preserve">criteria to curate vaccines</t>
   </si>
   <si>
-    <t xml:space="preserve">02_1_T2_create_QC_criteria</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">02_T2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">_1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">_create_QC_criteria</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">selected_doses</t>
@@ -122,7 +262,35 @@
     <t xml:space="preserve">curated vaccines</t>
   </si>
   <si>
-    <t xml:space="preserve">02_2_T3_apply_QC_exclusion_criteria</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">02_T3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">_2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">_apply_QC_exclusion_criteria</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Flowchart_QC_criteria</t>
@@ -137,7 +305,7 @@
     <t xml:space="preserve">exclusion criteria from PERSONS to the population of children</t>
   </si>
   <si>
-    <t xml:space="preserve">03_1_T2_create_exclusion_criteria</t>
+    <t xml:space="preserve">03_T2_1_create_exclusion_criteria</t>
   </si>
   <si>
     <t xml:space="preserve">D3_PERSONS OBSERVATION_PERIODS output_spells_category</t>
@@ -146,7 +314,35 @@
     <t xml:space="preserve">persons_doses</t>
   </si>
   <si>
-    <t xml:space="preserve">03_2_T2_merge_persons_concept</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">03_T2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">_2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">_merge_persons_concept</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">output_spells_category D3_selection_criteria D3_concepts_QC_criteria</t>
@@ -158,7 +354,35 @@
     <t xml:space="preserve">list of persons in the study population</t>
   </si>
   <si>
-    <t xml:space="preserve">04_1_T3_apply_exclusion_criteria</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">04_T3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">_1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">_apply_exclusion_criteria</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Flowchart_basic_exclusion_criteria</t>
@@ -983,7 +1207,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1021,6 +1245,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1096,88 +1326,92 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1265,1050 +1499,1050 @@
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
-      <selection pane="bottomRight" activeCell="G2" activeCellId="0" sqref="G2"/>
+      <selection pane="bottomRight" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="50.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="55.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="21.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="50.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="19.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="55.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="17.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.43"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+    <row r="1" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" s="4" customFormat="true" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="5" t="s">
+    <row r="2" s="5" customFormat="true" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="6" t="s">
+      <c r="C2" s="6"/>
+      <c r="D2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="7" t="s">
+      <c r="E2" s="7"/>
+      <c r="F2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" s="8" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
+    <row r="3" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
+    <row r="4" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="6" t="s">
+    <row r="5" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" s="8" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8" t="s">
+    <row r="6" s="9" customFormat="true" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="8" t="s">
+      <c r="C6" s="11"/>
+      <c r="D6" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" s="8" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8" t="s">
+    <row r="7" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="8" t="s">
+      <c r="C7" s="11"/>
+      <c r="D7" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="6" t="s">
+    <row r="8" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" s="8" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="8" t="s">
+    <row r="9" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" s="8" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="8" t="s">
+    <row r="10" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" s="6" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="6" t="s">
+    <row r="11" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="8" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="12" s="8" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="8" t="s">
+    <row r="12" s="9" customFormat="true" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="F12" s="10" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="13" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="6" t="s">
+    <row r="13" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="14" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="6" t="s">
+    <row r="14" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="F14" s="8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="15" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="6" t="s">
+    <row r="15" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="F15" s="8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="16" s="8" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="8" t="s">
+    <row r="16" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="F16" s="9" t="s">
+      <c r="F16" s="10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="17" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="6" t="s">
+    <row r="17" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="F17" s="8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="18" s="8" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="8" t="s">
+    <row r="18" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="F18" s="9" t="s">
+      <c r="F18" s="10" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="19" s="8" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="8" t="s">
+    <row r="19" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="F19" s="9" t="s">
+      <c r="F19" s="10" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="20" s="8" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="8" t="s">
+    <row r="20" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="F20" s="9" t="s">
+      <c r="F20" s="10" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="21" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="6" t="s">
+    <row r="21" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="F21" s="7" t="s">
+      <c r="F21" s="8" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="22" s="8" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="8" t="s">
+    <row r="22" s="9" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="F22" s="9" t="s">
+      <c r="F22" s="10" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="23" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="6" t="s">
+    <row r="23" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D23" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="F23" s="7" t="s">
+      <c r="F23" s="8" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="24" s="8" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="8" t="s">
+    <row r="24" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="F24" s="9" t="s">
+      <c r="F24" s="10" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="25" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="6" t="s">
+    <row r="25" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D25" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F25" s="7" t="s">
+      <c r="F25" s="8" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="26" s="8" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="8" t="s">
+    <row r="26" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="F26" s="9" t="s">
+      <c r="F26" s="10" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="27" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="6" t="s">
+    <row r="27" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="F27" s="7" t="s">
+      <c r="F27" s="8" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="28" s="8" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="8" t="s">
+    <row r="28" s="9" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C28" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="D28" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="F28" s="9" t="s">
+      <c r="F28" s="10" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="29" s="6" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="6" t="s">
+    <row r="29" s="7" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C29" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="D29" s="6" t="s">
+      <c r="D29" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="F29" s="7" t="s">
+      <c r="F29" s="8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="30" s="6" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="6" t="s">
+    <row r="30" s="7" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="C30" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="D30" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="F30" s="7" t="s">
+      <c r="F30" s="8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="31" s="6" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="6" t="s">
+    <row r="31" s="7" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="C31" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="D31" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="F31" s="7" t="s">
+      <c r="F31" s="8" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="C32" s="8"/>
-      <c r="D32" s="12" t="s">
+      <c r="C32" s="9"/>
+      <c r="D32" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="F32" s="9" t="s">
+      <c r="F32" s="10" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="C33" s="8"/>
-      <c r="D33" s="12" t="s">
+      <c r="C33" s="9"/>
+      <c r="D33" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="F33" s="9" t="s">
+      <c r="F33" s="10" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="34" s="6" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="6" t="s">
+    <row r="34" s="7" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="D34" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="F34" s="7" t="s">
+      <c r="F34" s="8" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="35" s="6" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="6" t="s">
+    <row r="35" s="7" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="D35" s="6" t="s">
+      <c r="D35" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="F35" s="7" t="s">
+      <c r="F35" s="8" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="8" t="s">
+      <c r="B36" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="C36" s="8"/>
-      <c r="D36" s="12" t="s">
+      <c r="C36" s="9"/>
+      <c r="D36" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="F36" s="9" t="s">
+      <c r="F36" s="10" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="8" t="s">
+      <c r="B37" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="C37" s="8"/>
-      <c r="D37" s="12" t="s">
+      <c r="C37" s="9"/>
+      <c r="D37" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="F37" s="9" t="s">
+      <c r="F37" s="10" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="38" s="13" customFormat="true" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="14" t="s">
+    <row r="38" s="15" customFormat="true" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="C38" s="14"/>
-      <c r="D38" s="13" t="s">
+      <c r="C38" s="16"/>
+      <c r="D38" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="F38" s="15" t="s">
+      <c r="F38" s="17" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="39" s="13" customFormat="true" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="14" t="s">
+    <row r="39" s="15" customFormat="true" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="C39" s="14"/>
-      <c r="D39" s="13" t="s">
+      <c r="C39" s="16"/>
+      <c r="D39" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="F39" s="15" t="s">
+      <c r="F39" s="17" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="40" s="8" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="8" t="s">
+    <row r="40" s="9" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="D40" s="8" t="s">
+      <c r="D40" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="F40" s="9" t="s">
+      <c r="F40" s="10" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="41" s="8" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="8" t="s">
+    <row r="41" s="9" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D41" s="8" t="s">
+      <c r="D41" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="F41" s="9" t="s">
+      <c r="F41" s="10" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="42" s="16" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="17" t="s">
+    <row r="42" s="18" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="C42" s="17"/>
-      <c r="D42" s="16" t="s">
+      <c r="C42" s="19"/>
+      <c r="D42" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="F42" s="18" t="s">
+      <c r="F42" s="20" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="43" s="8" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="8" t="s">
+    <row r="43" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="D43" s="8" t="s">
+      <c r="D43" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="F43" s="9" t="s">
+      <c r="F43" s="10" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="44" s="16" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="17" t="s">
+    <row r="44" s="18" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="C44" s="17"/>
-      <c r="D44" s="16" t="s">
+      <c r="C44" s="19"/>
+      <c r="D44" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="F44" s="18" t="s">
+      <c r="F44" s="20" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="45" s="16" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="17" t="s">
+    <row r="45" s="18" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="C45" s="17"/>
-      <c r="D45" s="16" t="s">
+      <c r="C45" s="19"/>
+      <c r="D45" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="F45" s="18" t="s">
+      <c r="F45" s="20" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="46" s="8" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="8" t="s">
+    <row r="46" s="9" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="D46" s="8" t="s">
+      <c r="D46" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="F46" s="9" t="s">
+      <c r="F46" s="10" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="47" s="8" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="8" t="s">
+    <row r="47" s="9" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="D47" s="8" t="s">
+      <c r="D47" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="F47" s="9" t="s">
+      <c r="F47" s="10" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="48" s="8" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="8" t="s">
+    <row r="48" s="9" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="D48" s="8" t="s">
+      <c r="D48" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="F48" s="9" t="s">
+      <c r="F48" s="10" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="49" s="8" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="8" t="s">
+    <row r="49" s="9" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B49" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="D49" s="8" t="s">
+      <c r="D49" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="F49" s="9" t="s">
+      <c r="F49" s="10" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="50" s="8" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="8" t="s">
+    <row r="50" s="9" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="D50" s="8" t="s">
+      <c r="D50" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="F50" s="9" t="s">
+      <c r="F50" s="10" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="51" s="8" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="8" t="s">
+    <row r="51" s="9" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="D51" s="8" t="s">
+      <c r="D51" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="F51" s="9" t="s">
+      <c r="F51" s="10" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="52" s="16" customFormat="true" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="17" t="s">
+    <row r="52" s="18" customFormat="true" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B52" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="C52" s="17"/>
-      <c r="D52" s="16" t="s">
+      <c r="C52" s="19"/>
+      <c r="D52" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="F52" s="18" t="s">
+      <c r="F52" s="20" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="53" s="16" customFormat="true" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="17" t="s">
+    <row r="53" s="18" customFormat="true" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B53" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="C53" s="17"/>
-      <c r="D53" s="16" t="s">
+      <c r="C53" s="19"/>
+      <c r="D53" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="F53" s="18" t="s">
+      <c r="F53" s="20" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="54" s="16" customFormat="true" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B54" s="17" t="s">
+    <row r="54" s="18" customFormat="true" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B54" s="19" t="s">
         <v>142</v>
       </c>
-      <c r="C54" s="17"/>
-      <c r="D54" s="16" t="s">
+      <c r="C54" s="19"/>
+      <c r="D54" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="F54" s="18" t="s">
+      <c r="F54" s="20" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="55" s="16" customFormat="true" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="17" t="s">
+    <row r="55" s="18" customFormat="true" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B55" s="19" t="s">
         <v>143</v>
       </c>
-      <c r="C55" s="17"/>
-      <c r="D55" s="16" t="s">
+      <c r="C55" s="19"/>
+      <c r="D55" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="F55" s="18" t="s">
+      <c r="F55" s="20" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="56" s="16" customFormat="true" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="17" t="s">
+    <row r="56" s="18" customFormat="true" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B56" s="19" t="s">
         <v>144</v>
       </c>
-      <c r="C56" s="17"/>
-      <c r="D56" s="16" t="s">
+      <c r="C56" s="19"/>
+      <c r="D56" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="F56" s="18" t="s">
+      <c r="F56" s="20" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="57" s="16" customFormat="true" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="17" t="s">
+    <row r="57" s="18" customFormat="true" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B57" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="C57" s="17"/>
-      <c r="D57" s="16" t="s">
+      <c r="C57" s="19"/>
+      <c r="D57" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="F57" s="18" t="s">
+      <c r="F57" s="20" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="58" s="16" customFormat="true" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B58" s="17" t="s">
+    <row r="58" s="18" customFormat="true" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B58" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="C58" s="17"/>
-      <c r="D58" s="16" t="s">
+      <c r="C58" s="19"/>
+      <c r="D58" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="F58" s="18" t="s">
+      <c r="F58" s="20" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="59" s="16" customFormat="true" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B59" s="17" t="s">
+    <row r="59" s="18" customFormat="true" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B59" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="C59" s="17"/>
-      <c r="D59" s="16" t="s">
+      <c r="C59" s="19"/>
+      <c r="D59" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="F59" s="18" t="s">
+      <c r="F59" s="20" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B60" s="8" t="s">
+      <c r="B60" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="C60" s="8"/>
-      <c r="D60" s="8" t="s">
+      <c r="C60" s="9"/>
+      <c r="D60" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="F60" s="9" t="s">
+      <c r="F60" s="10" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="61" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="6" t="s">
+    <row r="61" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B61" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="D61" s="6" t="s">
+      <c r="D61" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="F61" s="7" t="s">
+      <c r="F61" s="8" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B62" s="8" t="s">
+      <c r="B62" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="C62" s="8"/>
-      <c r="D62" s="8" t="s">
+      <c r="C62" s="9"/>
+      <c r="D62" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="F62" s="18" t="s">
+      <c r="F62" s="20" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="63" s="6" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B63" s="6" t="s">
+    <row r="63" s="7" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B63" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="D63" s="6" t="s">
+      <c r="D63" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="F63" s="7" t="s">
+      <c r="F63" s="8" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B64" s="0" t="s">
+      <c r="B64" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="D64" s="0" t="s">
+      <c r="D64" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="F64" s="1" t="s">
+      <c r="F64" s="2" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="65" s="6" customFormat="true" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B65" s="6" t="s">
+    <row r="65" s="7" customFormat="true" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B65" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="D65" s="6" t="s">
+      <c r="D65" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="F65" s="7" t="s">
+      <c r="F65" s="8" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="66" s="6" customFormat="true" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B66" s="6" t="s">
+    <row r="66" s="7" customFormat="true" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B66" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="D66" s="6" t="s">
+      <c r="D66" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="F66" s="7" t="s">
+      <c r="F66" s="8" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="67" s="6" customFormat="true" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B67" s="6" t="s">
+    <row r="67" s="7" customFormat="true" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B67" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="D67" s="6" t="s">
+      <c r="D67" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="F67" s="7" t="s">
+      <c r="F67" s="8" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="68" s="6" customFormat="true" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B68" s="6" t="s">
+    <row r="68" s="7" customFormat="true" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B68" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="D68" s="6" t="s">
+      <c r="D68" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="F68" s="7" t="s">
+      <c r="F68" s="8" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B69" s="0" t="s">
+      <c r="B69" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="D69" s="0" t="s">
+      <c r="D69" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="F69" s="9" t="s">
+      <c r="F69" s="10" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B70" s="0" t="s">
+      <c r="B70" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="D70" s="0" t="s">
+      <c r="D70" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="F70" s="9" t="s">
+      <c r="F70" s="10" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B71" s="0" t="s">
+      <c r="B71" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="D71" s="0" t="s">
+      <c r="D71" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="F71" s="9" t="s">
+      <c r="F71" s="10" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B72" s="0" t="s">
+      <c r="B72" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="D72" s="0" t="s">
+      <c r="D72" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="F72" s="9" t="s">
+      <c r="F72" s="10" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="73" s="6" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B73" s="6" t="s">
+    <row r="73" s="7" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B73" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="D73" s="6" t="s">
+      <c r="D73" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="F73" s="7" t="s">
+      <c r="F73" s="8" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="74" s="6" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B74" s="6" t="s">
+    <row r="74" s="7" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B74" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="D74" s="6" t="s">
+      <c r="D74" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="F74" s="7" t="s">
+      <c r="F74" s="8" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="75" s="6" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B75" s="6" t="s">
+    <row r="75" s="7" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B75" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="D75" s="6" t="s">
+      <c r="D75" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="F75" s="7" t="s">
+      <c r="F75" s="8" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="76" s="6" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B76" s="6" t="s">
+    <row r="76" s="7" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B76" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="D76" s="6" t="s">
+      <c r="D76" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="F76" s="7" t="s">
+      <c r="F76" s="8" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="315" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B77" s="0" t="s">
+      <c r="B77" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="C77" s="1" t="s">
+      <c r="C77" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="D77" s="0" t="s">
+      <c r="D77" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="F77" s="1" t="s">
+      <c r="F77" s="2" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B78" s="0" t="s">
+      <c r="B78" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="C78" s="0" t="s">
+      <c r="C78" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="D78" s="0" t="s">
+      <c r="D78" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="F78" s="1" t="s">
+      <c r="F78" s="2" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="79" s="6" customFormat="true" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B79" s="6" t="s">
+    <row r="79" s="7" customFormat="true" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B79" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="C79" s="6" t="s">
+      <c r="C79" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="D79" s="6" t="s">
+      <c r="D79" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="F79" s="7" t="s">
+      <c r="F79" s="8" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B80" s="0" t="s">
+      <c r="B80" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="D80" s="0" t="s">
+      <c r="D80" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="F80" s="9" t="s">
+      <c r="F80" s="10" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="81" s="6" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B81" s="6" t="s">
+    <row r="81" s="7" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B81" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="D81" s="6" t="s">
+      <c r="D81" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="F81" s="7" t="s">
+      <c r="F81" s="8" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B82" s="0" t="s">
+      <c r="B82" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="D82" s="0" t="s">
+      <c r="D82" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="F82" s="1" t="s">
+      <c r="F82" s="2" t="s">
         <v>193</v>
       </c>
     </row>
@@ -2331,29 +2565,29 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D15 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="21" t="s">
         <v>198</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="21" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="11" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="11" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>